<commit_message>
Allow blank banner. New changes to language captions
</commit_message>
<xml_diff>
--- a/acharyan_captions_english.xlsx
+++ b/acharyan_captions_english.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\Parampara_Poster\parampara_poster_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6352C534-305D-4F42-88D2-D4651C55DDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01893A16-857C-4A66-B010-04F30F47AC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45920" yWindow="1810" windowWidth="27580" windowHeight="19070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41960" yWindow="5480" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acharyan_captions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>Sri Parakāla Mata Ācāryas</t>
   </si>
@@ -228,19 +228,19 @@
     <t>Sridevi</t>
   </si>
   <si>
-    <t>Sri Parakāla Swāmy Maṭham Guru Parampara</t>
-  </si>
-  <si>
-    <t>Sri Parakāla Swāmy Maṭham Āchāryas</t>
-  </si>
-  <si>
-    <t>Sri Parakāla Swāmy Maṭham – The Eternal Lineage of the Sri Vedānta Deśika</t>
-  </si>
-  <si>
-    <t>Lineage of the Brahmatantra Swatantra Swamys</t>
-  </si>
-  <si>
     <t>Kidambi Rāmānuja Piḷḷān</t>
+  </si>
+  <si>
+    <t>Sri Brahmatantra Swatantra Parakala Swāmy Mutt Acharyas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maṭham </t>
+  </si>
+  <si>
+    <t>Sri Parakāla Swāmy Mutt – The Eternal Lineage of the Sri Vedānta Deśika</t>
+  </si>
+  <si>
+    <t>Sri Parakāla Swāmy Mutt Guru Parampara</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1064,7 +1064,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -1135,15 +1135,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="64.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -1151,15 +1154,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1167,27 +1173,30 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>66</v>
       </c>
       <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Name changes and cleanup
</commit_message>
<xml_diff>
--- a/acharyan_captions_english.xlsx
+++ b/acharyan_captions_english.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\Parampara_Poster\parampara_poster_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01893A16-857C-4A66-B010-04F30F47AC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FAD764-8F29-417F-B0C7-B7501459B188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41960" yWindow="5480" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="4140" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acharyan_captions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Sri Parakāla Mata Ācāryas</t>
   </si>
@@ -30,111 +30,9 @@
     <t>Sri Brahmatantra Swatantra Maha Deśikan (1359 – 1386)</t>
   </si>
   <si>
-    <t>Sri Dviteeya (Vātsya Vedānta Rāmānuja) Brahmatantra Swatantra Mahā Deśikan (1386 – 1394)</t>
-  </si>
-  <si>
-    <t>Sri Tṛtīya (Srinivāsa) Brahmatantra Swatantra Mahā Deśikan (1394 – 1406)</t>
-  </si>
-  <si>
-    <t>Sri Parakāla Brahmatantra Swatantra Mahā Deśikan (1406 – 1424)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Rāmānuja Brahmatantra Swatantra Mahā Deśikan (1424 – 1440)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Brahmatantra Swatantra Mahā Deśikan (1440 – 1460)</t>
-  </si>
-  <si>
-    <t>Sri Nārāyaṇa Yogindra Brahmatantra Swatantra Mahā Deśikan (1460 – 1482)</t>
-  </si>
-  <si>
-    <t>Sri Raṅgarāja Yogindra Brahmatantra Swatantra Mahā Deśikan (1482 – 1498)</t>
-  </si>
-  <si>
-    <t>Sri Chaturtha Brahmatantra Swatantra Mahā Deśikan (1498 – 1517)</t>
-  </si>
-  <si>
-    <t>Sri Yatirāja Brahmatantra Swatantra Mahā Deśikan (1517 – 1535)</t>
-  </si>
-  <si>
-    <t>Sri Varada Brahmatantra Swatantra Mahā Deśikan (1535 – 1552)</t>
-  </si>
-  <si>
-    <t>Sri Parāṅkuśa Brahmatantra Swatantra Mahā Deśikan (1552 – 1567)</t>
-  </si>
-  <si>
-    <t>Sri Kavitārkika Siṃha Brahmatantra Swatantra Mahā Deśikan (1567 – 1583)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Yathivarya Brahmatantra Swatantra Mahā Deśikan (1583 – 1607)</t>
-  </si>
-  <si>
-    <t>Sri Jñānābdi Brahmatantra Swatantra Mahā Deśikan (1607 – 1618)</t>
-  </si>
-  <si>
-    <t>Sri Vīrarāghava Yogindra Brahmatantra Swatantra Mahā Deśikan (1618 – 1640)</t>
-  </si>
-  <si>
-    <t>Sri Varada Vedānta Brahmatantra Swatantra Mahā Deśikan (1640 – 1652)</t>
-  </si>
-  <si>
-    <t>Sri Varāha Brahmatantra Swatantra Mahā Deśikan (1652 – 1663)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Lakṣmaṇa Brahmatantra Swatantra Mahā Deśikan (1663 – 1673)</t>
-  </si>
-  <si>
-    <t>Sri Varada Vedānta Yogīndra Brahmatantra Swatantra Mahā Deśikan (1673 – 1677)</t>
-  </si>
-  <si>
-    <t>Sri Maha Parakāla Brahmatantra Swatantra Mahā Deśikan (1676 – 1738)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Brahmatantra Swatantra Parakāla Mahā Deśikan (1738 – 1751)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Brahmatantra Swatantra Parakāla Mahā Deśikan (1750 – 1770)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Srinivāsa Brahmatantra Swatantra Parakāla Mahā Deśikan (1770 – 1772)</t>
-  </si>
-  <si>
     <t>Sri Rāmānuja Brahmatantra Swatantra Mahā Parakāla Deśikan (1772 – 1810)</t>
   </si>
   <si>
-    <t>Sri Ghantāvatāra Brahmatantra Swatantra Parakāla Mahā Deśikan (1810 – 1829)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Brahmatantra Swatantra Parakāla Mahā Deśikan (1829 – 1836)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Brahmatantra Swatantra Parakāla Mahā Deśikan (1836 – 1861)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Deśikendra Brahmatantra Swatantra Parakāla Mahā Deśikan (1861 – 1873)</t>
-  </si>
-  <si>
-    <t>Sri Raṅganātha Brahmatantra Swatantra Parakāla Mahā Deśikan (1873 – 1885)</t>
-  </si>
-  <si>
-    <t>Sri Kṛṣṇa Brahmatantra Swatantra Parakāla Mahā Deśikan (1885 – 1915)</t>
-  </si>
-  <si>
-    <t>Sri Vāgīśa Brahmatantra Swatantra Parakāla Mahā Deśikan (1915 – 1925)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Raṅganātha Brahmatantra Swatantra Parakāla Mahā Deśikan (1925 – 1967)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Srinivāsa Brahmatantra Swatantra Parakāla Mahā Deśikan (1967 – 1972)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Rāmānuja Brahmatantra Swatantra Parakāla Mahā Deśikan (1972 – 1992)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Vāgīśa Brahmatantra Swatantra Parakāla Mahā Deśikan (1992 – present)</t>
-  </si>
-  <si>
     <t>SL NO</t>
   </si>
   <si>
@@ -195,9 +93,6 @@
     <t>Kidambi Appuḷḷār</t>
   </si>
   <si>
-    <t>Nigamānta Mahā Deśikan</t>
-  </si>
-  <si>
     <t>Kumāra Varadāchārya</t>
   </si>
   <si>
@@ -234,13 +129,115 @@
     <t>Sri Brahmatantra Swatantra Parakala Swāmy Mutt Acharyas</t>
   </si>
   <si>
-    <t xml:space="preserve"> Maṭham </t>
-  </si>
-  <si>
     <t>Sri Parakāla Swāmy Mutt – The Eternal Lineage of the Sri Vedānta Deśika</t>
   </si>
   <si>
-    <t>Sri Parakāla Swāmy Mutt Guru Parampara</t>
+    <t>Nigamānta Mahādeśikan</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Rāmānuja Brahmatantra Swatantra Mahādeśikan (1424 – 1440)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Brahmatantra Swatantra Mahādeśikan (1440 – 1460)</t>
+  </si>
+  <si>
+    <t>Sri Nārāyaṇa Yogindra Brahmatantra Swatantra Mahādeśikan (1460 – 1482)</t>
+  </si>
+  <si>
+    <t>Sri Raṅgarāja Yogindra Brahmatantra Swatantra Mahādeśikan (1482 – 1498)</t>
+  </si>
+  <si>
+    <t>Sri Chaturtha Brahmatantra Swatantra Mahādeśikan (1498 – 1517)</t>
+  </si>
+  <si>
+    <t>Sri Yatirāja Brahmatantra Swatantra Mahādeśikan (1517 – 1535)</t>
+  </si>
+  <si>
+    <t>Sri Varada Brahmatantra Swatantra Mahādeśikan (1535 – 1552)</t>
+  </si>
+  <si>
+    <t>Sri Parāṅkuśa Brahmatantra Swatantra Mahādeśikan (1552 – 1567)</t>
+  </si>
+  <si>
+    <t>Sri Kavitārkika Siṃha Brahmatantra Swatantra Mahādeśikan (1567 – 1583)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Yathivarya Brahmatantra Swatantra Mahādeśikan (1583 – 1607)</t>
+  </si>
+  <si>
+    <t>Sri Jñānābdi Brahmatantra Swatantra Mahādeśikan (1607 – 1618)</t>
+  </si>
+  <si>
+    <t>Sri Vīrarāghava Yogindra Brahmatantra Swatantra Mahādeśikan (1618 – 1640)</t>
+  </si>
+  <si>
+    <t>Sri Varada Vedānta Brahmatantra Swatantra Mahādeśikan (1640 – 1652)</t>
+  </si>
+  <si>
+    <t>Sri Varāha Brahmatantra Swatantra Mahādeśikan (1652 – 1663)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Lakṣmaṇa Brahmatantra Swatantra Mahādeśikan (1663 – 1673)</t>
+  </si>
+  <si>
+    <t>Sri Varada Vedānta Yogīndra Brahmatantra Swatantra Mahādeśikan (1673 – 1677)</t>
+  </si>
+  <si>
+    <t>Sri Maha Parakāla Brahmatantra Swatantra Mahādeśikan (1676 – 1738)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Brahmatantra Swatantra Parakāla Mahādeśikan (1738 – 1751)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Brahmatantra Swatantra Parakāla Mahādeśikan (1750 – 1770)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Srinivāsa Brahmatantra Swatantra Parakāla Mahādeśikan (1770 – 1772)</t>
+  </si>
+  <si>
+    <t>Sri Ghantāvatāra Brahmatantra Swatantra Parakāla Mahādeśikan (1810 – 1829)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Brahmatantra Swatantra Parakāla Mahādeśikan (1829 – 1836)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Brahmatantra Swatantra Parakāla Mahādeśikan (1836 – 1861)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Deśikendra Brahmatantra Swatantra Parakāla Mahādeśikan (1861 – 1873)</t>
+  </si>
+  <si>
+    <t>Sri Raṅganātha Brahmatantra Swatantra Parakāla Mahādeśikan (1873 – 1885)</t>
+  </si>
+  <si>
+    <t>Sri Kṛṣṇa Brahmatantra Swatantra Parakāla Mahādeśikan (1885 – 1915)</t>
+  </si>
+  <si>
+    <t>Sri Vāgīśa Brahmatantra Swatantra Parakāla Mahādeśikan (1915 – 1925)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Raṅganātha Brahmatantra Swatantra Parakāla Mahādeśikan (1925 – 1967)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Srinivāsa Brahmatantra Swatantra Parakāla Mahādeśikan (1967 – 1972)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Rāmānuja Brahmatantra Swatantra Parakāla Mahādeśikan (1972 – 1992)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Vāgīśa Brahmatantra Swatantra Parakāla Mahādeśikan (1992 – present)</t>
+  </si>
+  <si>
+    <t>Sri Dviteeya (Vātsya Vedānta Rāmānuja) Brahmatantra Swatantra Mahādeśikan (1386 – 1394)</t>
+  </si>
+  <si>
+    <t>Sri Tṛtīya (Srinivāsa) Brahmatantra Swatantra Mahādeśikan (1394 – 1406)</t>
+  </si>
+  <si>
+    <t>Sri Parakāla Brahmatantra Swatantra Mahādeśikan (1406 – 1424)</t>
+  </si>
+  <si>
+    <t>Sri Brahmatantra Swatantra Parakala Swāmy Guru Parampara</t>
   </si>
 </sst>
 </file>
@@ -582,7 +579,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -604,7 +603,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -612,7 +611,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -620,7 +619,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -628,7 +627,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -636,7 +635,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -644,7 +643,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -652,7 +651,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -660,7 +659,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -668,7 +667,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -676,7 +675,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -684,7 +683,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -692,7 +691,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -700,7 +699,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -708,7 +707,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -716,7 +715,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -724,7 +723,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -732,7 +731,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -740,7 +739,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -748,7 +747,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -756,7 +755,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -764,7 +763,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -772,7 +771,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -780,7 +779,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -788,7 +787,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -796,7 +795,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -804,7 +803,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -812,7 +811,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -820,7 +819,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -828,7 +827,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -836,7 +835,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -844,7 +843,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -852,7 +851,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -860,7 +859,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -868,7 +867,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -876,7 +875,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -889,7 +888,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -901,16 +900,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -918,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -929,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -940,7 +939,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -951,7 +950,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -962,7 +961,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -973,7 +972,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -984,7 +983,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -995,7 +994,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1006,7 +1005,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -1017,13 +1016,13 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1031,7 +1030,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1042,7 +1041,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -1053,7 +1052,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D14">
         <v>11</v>
@@ -1064,7 +1063,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -1075,7 +1074,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>12</v>
@@ -1086,7 +1085,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="D17">
         <v>12</v>
@@ -1097,7 +1096,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D18">
         <v>13</v>
@@ -1108,13 +1107,13 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D19">
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1122,7 +1121,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="D20">
         <v>15</v>
@@ -1135,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1146,58 +1145,49 @@
     <col min="2" max="2" width="64.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug in time range split fix. Also language fixes
</commit_message>
<xml_diff>
--- a/acharyan_captions_english.xlsx
+++ b/acharyan_captions_english.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\Parampara_Poster\parampara_poster_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FAD764-8F29-417F-B0C7-B7501459B188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CCDB03-9B13-4FF0-A49D-3ED3DA63AE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="4140" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38460" yWindow="1280" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acharyan_captions" sheetId="1" r:id="rId1"/>
@@ -126,12 +126,6 @@
     <t>Kidambi Rāmānuja Piḷḷān</t>
   </si>
   <si>
-    <t>Sri Brahmatantra Swatantra Parakala Swāmy Mutt Acharyas</t>
-  </si>
-  <si>
-    <t>Sri Parakāla Swāmy Mutt – The Eternal Lineage of the Sri Vedānta Deśika</t>
-  </si>
-  <si>
     <t>Nigamānta Mahādeśikan</t>
   </si>
   <si>
@@ -237,7 +231,13 @@
     <t>Sri Parakāla Brahmatantra Swatantra Mahādeśikan (1406 – 1424)</t>
   </si>
   <si>
-    <t>Sri Brahmatantra Swatantra Parakala Swāmy Guru Parampara</t>
+    <t>Sri Brahmatantra Svatantra Parakāla Swāmi Mutt Guru Paramparā</t>
+  </si>
+  <si>
+    <t>Sri Brahmatantra Svatantra Parakāla Swāmi Mutt Ācāryas</t>
+  </si>
+  <si>
+    <t>Sri Parakāla Swāmi Mutt – The Eternal Lineage of Sri Vedānta Deśika</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +603,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -611,7 +611,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -619,7 +619,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -627,7 +627,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -635,7 +635,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -643,7 +643,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -651,7 +651,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -659,7 +659,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -667,7 +667,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -675,7 +675,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -683,7 +683,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -691,7 +691,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -699,7 +699,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -707,7 +707,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -715,7 +715,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -723,7 +723,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -731,7 +731,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -739,7 +739,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -747,7 +747,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -755,7 +755,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -763,7 +763,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -771,7 +771,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -779,7 +779,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -795,7 +795,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -803,7 +803,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -811,7 +811,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -819,7 +819,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -827,7 +827,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -835,7 +835,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -843,7 +843,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -851,7 +851,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -859,7 +859,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -867,7 +867,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -875,7 +875,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1107,7 +1107,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19">
         <v>14</v>
@@ -1136,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1158,7 +1158,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1174,7 +1174,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1187,7 +1187,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Text fixes in English
</commit_message>
<xml_diff>
--- a/acharyan_captions_english.xlsx
+++ b/acharyan_captions_english.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\Parampara_Poster\parampara_poster_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CCDB03-9B13-4FF0-A49D-3ED3DA63AE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165B9F41-D542-4F83-AD5A-0D8A6D4B21A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38460" yWindow="1280" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,12 +45,6 @@
     <t>ENHANCE</t>
   </si>
   <si>
-    <t>Sri Lakshmi Hayagriva</t>
-  </si>
-  <si>
-    <t>Sri Vishvaksena</t>
-  </si>
-  <si>
     <t>Swāmi Nammāḷvār</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>Tirukkurugai Pirān Piḷḷān</t>
   </si>
   <si>
-    <t xml:space="preserve"> Kidambi Ācchan</t>
-  </si>
-  <si>
     <t>Engalāḷvān</t>
   </si>
   <si>
@@ -120,9 +111,6 @@
     <t>M5</t>
   </si>
   <si>
-    <t>Sridevi</t>
-  </si>
-  <si>
     <t>Kidambi Rāmānuja Piḷḷān</t>
   </si>
   <si>
@@ -231,13 +219,25 @@
     <t>Sri Parakāla Brahmatantra Swatantra Mahādeśikan (1406 – 1424)</t>
   </si>
   <si>
-    <t>Sri Brahmatantra Svatantra Parakāla Swāmi Mutt Guru Paramparā</t>
-  </si>
-  <si>
-    <t>Sri Brahmatantra Svatantra Parakāla Swāmi Mutt Ācāryas</t>
-  </si>
-  <si>
     <t>Sri Parakāla Swāmi Mutt – The Eternal Lineage of Sri Vedānta Deśika</t>
+  </si>
+  <si>
+    <t>Sri Brahmatantra Swatantra Parakāla Swāmi Mutt Guru Paramparā</t>
+  </si>
+  <si>
+    <t>Sri Brahmatantra Swatantra Parakāla Swāmi Mutt Ācāryas</t>
+  </si>
+  <si>
+    <t>Śrīdevī</t>
+  </si>
+  <si>
+    <t>Śrī Lakṣmī Hayagrīva</t>
+  </si>
+  <si>
+    <t>Śrī Viśvaksena</t>
+  </si>
+  <si>
+    <t>Kidambi Āccān</t>
   </si>
 </sst>
 </file>
@@ -273,8 +273,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -611,7 +614,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -619,7 +622,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -627,7 +630,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -635,7 +638,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -643,7 +646,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -651,7 +654,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -659,7 +662,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -667,7 +670,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -675,7 +678,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -683,7 +686,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -691,7 +694,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -699,7 +702,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -707,7 +710,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -715,7 +718,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -723,7 +726,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -731,7 +734,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -739,7 +742,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -747,7 +750,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -755,7 +758,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -763,7 +766,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -771,7 +774,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -779,7 +782,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -795,7 +798,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -803,7 +806,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -811,7 +814,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -819,7 +822,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -827,7 +830,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -835,7 +838,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -843,7 +846,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -851,7 +854,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -859,7 +862,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -867,7 +870,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -875,7 +878,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -888,242 +891,243 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="3" max="3" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
+    <col min="4" max="4" width="20.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D9" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D11" s="1">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="D11">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D14" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D16" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="D17" s="1">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
         <v>19</v>
       </c>
-      <c r="D14">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="D18" s="1">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
         <v>20</v>
       </c>
-      <c r="D16">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19">
-        <v>14</v>
-      </c>
-      <c r="E19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>15</v>
       </c>
     </row>
@@ -1137,57 +1141,58 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
     <col min="2" max="2" width="64.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>